<commit_message>
Actualización de registro de Deudos
</commit_message>
<xml_diff>
--- a/bd/scot.xlsx
+++ b/bd/scot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JairoLaguna\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JairoLaguna\Desktop\scot\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F9DDE98-6013-48E6-ABE6-95F836AB7893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEA2CA41-8DE3-4D5D-BE5B-A900A2580DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{C6115F0C-3CF3-415B-A17C-C60CFFE12FD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{B5D3DCC6-E143-47E6-BCA4-9BE9C3725A22}"/>
   </bookViews>
   <sheets>
     <sheet name="scot" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="623">
   <si>
     <t>idBarrio</t>
   </si>
@@ -1207,12 +1207,12 @@
     <t>estadoFierro</t>
   </si>
   <si>
+    <t>INACTIVO</t>
+  </si>
+  <si>
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>INACTIVO</t>
-  </si>
-  <si>
     <t>codIBI</t>
   </si>
   <si>
@@ -1222,6 +1222,24 @@
     <t>ubicacion</t>
   </si>
   <si>
+    <t>construccion</t>
+  </si>
+  <si>
+    <t>tipoIBI</t>
+  </si>
+  <si>
+    <t>uso</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>barrido</t>
+  </si>
+  <si>
+    <t>valorCatastral</t>
+  </si>
+  <si>
     <t>finca</t>
   </si>
   <si>
@@ -1234,12 +1252,6 @@
     <t>asiento</t>
   </si>
   <si>
-    <t>valorCatastral</t>
-  </si>
-  <si>
-    <t>construccion</t>
-  </si>
-  <si>
     <t>estadoIBI</t>
   </si>
   <si>
@@ -1249,12 +1261,21 @@
     <t>ESQUINA SUR-ESTE DEL C/S BUENA VIDA</t>
   </si>
   <si>
+    <t>CASA</t>
+  </si>
+  <si>
+    <t>URBANO</t>
+  </si>
+  <si>
+    <t>CASA DE HABITACION</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>Finca 1</t>
   </si>
   <si>
-    <t>CASA</t>
-  </si>
-  <si>
     <t>0604U000012455</t>
   </si>
   <si>
@@ -1282,6 +1303,18 @@
     <t>IGLESIA RESTAURACION</t>
   </si>
   <si>
+    <t>0604U003011111</t>
+  </si>
+  <si>
+    <t>JINOTEGA NORTE</t>
+  </si>
+  <si>
+    <t>CASA DESHABITADA</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>sector</t>
   </si>
   <si>
@@ -1321,24 +1354,27 @@
     <t>CV8889</t>
   </si>
   <si>
+    <t>LIBRE</t>
+  </si>
+  <si>
+    <t>1.5x2.0m</t>
+  </si>
+  <si>
+    <t>CV1005</t>
+  </si>
+  <si>
+    <t>CV2006</t>
+  </si>
+  <si>
+    <t>CV1019</t>
+  </si>
+  <si>
+    <t>CV1021</t>
+  </si>
+  <si>
     <t>OCUPADO</t>
   </si>
   <si>
-    <t>1.5x2.0m</t>
-  </si>
-  <si>
-    <t>CV1005</t>
-  </si>
-  <si>
-    <t>CV2006</t>
-  </si>
-  <si>
-    <t>CV1019</t>
-  </si>
-  <si>
-    <t>CV1021</t>
-  </si>
-  <si>
     <t>CV3055</t>
   </si>
   <si>
@@ -1357,9 +1393,6 @@
     <t>CV3056</t>
   </si>
   <si>
-    <t>LIBRE</t>
-  </si>
-  <si>
     <t>SUR-ESTE</t>
   </si>
   <si>
@@ -1393,7 +1426,7 @@
     <t>CN1020</t>
   </si>
   <si>
-    <t>2M X 3M</t>
+    <t>2M X 3.5M</t>
   </si>
   <si>
     <t>Terreno en espera</t>
@@ -1426,28 +1459,25 @@
     <t>mesPago</t>
   </si>
   <si>
-    <t>241-092888-0002F</t>
+    <t>241-201076-0000P</t>
   </si>
   <si>
     <t>NULL</t>
   </si>
   <si>
-    <t>401-071690-0002Q</t>
-  </si>
-  <si>
-    <t>241-052782-0001C</t>
-  </si>
-  <si>
-    <t>241-061483-0001M</t>
+    <t>241-151090-0002C</t>
+  </si>
+  <si>
+    <t>001-291275-0008Q</t>
   </si>
   <si>
     <t>242-073079-0009P</t>
   </si>
   <si>
-    <t>001-111190-0004A</t>
-  </si>
-  <si>
-    <t>241-040381-0001G</t>
+    <t>001-150855-0023S</t>
+  </si>
+  <si>
+    <t>241-151088-0000L</t>
   </si>
   <si>
     <t>parametro</t>
@@ -1495,15 +1525,12 @@
     <t>codTA</t>
   </si>
   <si>
-    <t>tipoTA</t>
+    <t>tipoVivienda</t>
   </si>
   <si>
     <t>estadoTA</t>
   </si>
   <si>
-    <t>URBANO</t>
-  </si>
-  <si>
     <t>RURAL</t>
   </si>
   <si>
@@ -1513,30 +1540,18 @@
     <t>codEntidad</t>
   </si>
   <si>
-    <t>241-151090-0002C</t>
-  </si>
-  <si>
-    <t>241-201076-0000P</t>
-  </si>
-  <si>
-    <t>001-291275-0008Q</t>
-  </si>
-  <si>
-    <t>TA</t>
-  </si>
-  <si>
-    <t>001-150855-0023S</t>
-  </si>
-  <si>
     <t>LOTE</t>
   </si>
   <si>
-    <t>241-151088-0000L</t>
+    <t>CV8890-B</t>
   </si>
   <si>
     <t>241-151155-0000G</t>
   </si>
   <si>
+    <t>0604R410002950-B</t>
+  </si>
+  <si>
     <t>idUsuario</t>
   </si>
   <si>
@@ -1807,7 +1822,7 @@
     <t>ORUGAAMAD55@GMAIL.COM</t>
   </si>
   <si>
-    <t>8825-1570</t>
+    <t>8825-1575</t>
   </si>
   <si>
     <t>ALMAIRIS</t>
@@ -1852,41 +1867,35 @@
     <t>CUOTA</t>
   </si>
   <si>
-    <t>DEUDOS</t>
+    <t>DEUDO</t>
   </si>
   <si>
     <t>DISTRITO</t>
   </si>
   <si>
-    <t>LOTES</t>
-  </si>
-  <si>
     <t>MULTA</t>
   </si>
   <si>
+    <t>PAGO</t>
+  </si>
+  <si>
+    <t>PARAMETRO</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
     <t>TRIBUTO</t>
   </si>
   <si>
-    <t>PARAMETROS</t>
-  </si>
-  <si>
-    <t>SECTORES</t>
-  </si>
-  <si>
-    <t>TREN DE ASEO (TA)</t>
-  </si>
-  <si>
-    <t>USUARIOS</t>
-  </si>
-  <si>
-    <t>TRIBUTOS</t>
+    <t>SECTOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2017,15 +2026,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2406,14 +2406,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2768,41 +2768,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BB9B12-93A6-4D97-B475-C7C0219DAAED}">
-  <dimension ref="A1:M313"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76849C63-1BCF-47EF-97C3-3BAF2A9DFF57}">
+  <dimension ref="A1:N326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="C305" sqref="C305"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="C269" sqref="C269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5696,16 +5694,23 @@
         <v>314</v>
       </c>
     </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="3"/>
+      <c r="B173" s="3"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="3"/>
+      <c r="E173" s="3"/>
+    </row>
     <row r="174" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A174" s="4" t="s">
-        <v>608</v>
+      <c r="A174" s="7" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
+      <c r="A175" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="B175" s="4" t="s">
         <v>354</v>
       </c>
     </row>
@@ -5733,16 +5738,21 @@
         <v>357</v>
       </c>
     </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="3"/>
+      <c r="B179" s="3"/>
+    </row>
     <row r="180" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A180" s="4" t="s">
-        <v>482</v>
-      </c>
+      <c r="A180" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="B180" s="3"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
+      <c r="A181" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B181" s="3" t="s">
+      <c r="B181" s="4" t="s">
         <v>359</v>
       </c>
     </row>
@@ -5762,22 +5772,27 @@
         <v>361</v>
       </c>
     </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="3"/>
+      <c r="B184" s="3"/>
+    </row>
     <row r="185" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A185" s="4" t="s">
-        <v>609</v>
-      </c>
+      <c r="A185" s="8" t="s">
+        <v>614</v>
+      </c>
+      <c r="B185" s="3"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
+      <c r="A186" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B186" s="3" t="s">
+      <c r="B186" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="C186" s="3" t="s">
+      <c r="C186" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="D186" s="3" t="s">
+      <c r="D186" s="4" t="s">
         <v>365</v>
       </c>
     </row>
@@ -5788,7 +5803,7 @@
       <c r="B187" s="2">
         <v>3</v>
       </c>
-      <c r="C187" s="5">
+      <c r="C187" s="6">
         <v>45418</v>
       </c>
       <c r="D187" s="2">
@@ -5796,31 +5811,34 @@
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C188" s="1"/>
+      <c r="A188" s="3"/>
+      <c r="B188" s="3"/>
+      <c r="C188" s="9"/>
+      <c r="D188" s="3"/>
     </row>
     <row r="189" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A189" s="4" t="s">
-        <v>610</v>
+      <c r="A189" s="7" t="s">
+        <v>615</v>
       </c>
       <c r="C189" s="1"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="3" t="s">
+      <c r="A190" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="B190" s="3" t="s">
+      <c r="B190" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="C190" s="3" t="s">
+      <c r="C190" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="D190" s="3" t="s">
+      <c r="D190" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="E190" s="3" t="s">
+      <c r="E190" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="F190" s="3" t="s">
+      <c r="F190" s="4" t="s">
         <v>371</v>
       </c>
     </row>
@@ -5837,7 +5855,7 @@
       <c r="D191" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E191" s="5">
+      <c r="E191" s="6">
         <v>23935</v>
       </c>
       <c r="F191" s="2" t="s">
@@ -5857,7 +5875,7 @@
       <c r="D192" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="E192" s="5">
+      <c r="E192" s="6">
         <v>29336</v>
       </c>
       <c r="F192" s="2" t="s">
@@ -5877,7 +5895,7 @@
       <c r="D193" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="E193" s="5">
+      <c r="E193" s="6">
         <v>36114</v>
       </c>
       <c r="F193" s="2" t="s">
@@ -5897,7 +5915,7 @@
       <c r="D194" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E194" s="5">
+      <c r="E194" s="6">
         <v>21272</v>
       </c>
       <c r="F194" s="2" t="s">
@@ -5917,7 +5935,7 @@
       <c r="D195" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="E195" s="5">
+      <c r="E195" s="6">
         <v>20320</v>
       </c>
       <c r="F195" s="2" t="s">
@@ -5937,7 +5955,7 @@
       <c r="D196" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E196" s="5">
+      <c r="E196" s="6">
         <v>33213</v>
       </c>
       <c r="F196" s="2" t="s">
@@ -5945,28 +5963,24 @@
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="6"/>
-      <c r="B197" s="6"/>
-      <c r="C197" s="6"/>
-      <c r="D197" s="6"/>
-      <c r="E197" s="7"/>
-      <c r="F197" s="6"/>
+      <c r="A197" s="3"/>
+      <c r="B197" s="3"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="3"/>
+      <c r="E197" s="9"/>
+      <c r="F197" s="3"/>
     </row>
     <row r="198" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A198" s="9" t="s">
-        <v>611</v>
-      </c>
-      <c r="B198" s="6"/>
-      <c r="C198" s="6"/>
-      <c r="D198" s="6"/>
-      <c r="E198" s="7"/>
-      <c r="F198" s="6"/>
+      <c r="A198" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="E198" s="1"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="B199" s="3" t="s">
+      <c r="B199" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6042,7 +6056,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>10</v>
       </c>
@@ -6050,151 +6064,145 @@
         <v>277</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A210" s="6"/>
-      <c r="B210" s="6"/>
-    </row>
-    <row r="211" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A211" s="9" t="s">
-        <v>537</v>
-      </c>
-      <c r="B211" s="6"/>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A212" s="3" t="s">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A210" s="3"/>
+      <c r="B210" s="3"/>
+    </row>
+    <row r="211" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A211" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="B211" s="3"/>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A212" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B212" s="3" t="s">
+      <c r="B212" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="C212" s="3" t="s">
+      <c r="C212" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="D212" s="3" t="s">
+      <c r="D212" s="4" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>9874</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C213" s="5">
+      <c r="C213" s="6">
         <v>45418</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>1152</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C214" s="5">
-        <v>45418</v>
+      <c r="C214" s="6">
+        <v>45413</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>9156</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C215" s="5">
+      <c r="C215" s="6">
         <v>45414</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A216" s="6"/>
-      <c r="B216" s="6"/>
-      <c r="C216" s="7"/>
-      <c r="D216" s="6"/>
-    </row>
-    <row r="217" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A217" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="C217" s="1"/>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A218" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C216" s="6">
+        <v>45476</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A217" s="3"/>
+      <c r="B217" s="3"/>
+      <c r="C217" s="9"/>
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A218" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C218" s="1"/>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A219" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="B218" s="3" t="s">
+      <c r="B219" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="C218" s="3" t="s">
+      <c r="C219" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="D218" s="3" t="s">
+      <c r="D219" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="E218" s="3" t="s">
+      <c r="E219" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F218" s="3" t="s">
+      <c r="F219" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="G218" s="3" t="s">
+      <c r="G219" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="H218" s="3" t="s">
+      <c r="H219" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="I218" s="3" t="s">
+      <c r="I219" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="J218" s="3" t="s">
+      <c r="J219" s="4" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A219" s="2">
+      <c r="K219" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="L219" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="M219" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="N219" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
         <v>1</v>
-      </c>
-      <c r="B219" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D219" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="E219" s="2">
-        <v>1</v>
-      </c>
-      <c r="F219" s="2">
-        <v>1</v>
-      </c>
-      <c r="G219" s="2">
-        <v>1</v>
-      </c>
-      <c r="H219" s="2">
-        <v>100000</v>
-      </c>
-      <c r="I219" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="J219" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A220" s="2">
-        <v>2</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>411</v>
@@ -6205,52 +6213,90 @@
       <c r="D220" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="E220" s="2">
+      <c r="E220" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G220" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H220" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I220" s="2">
+        <v>100000</v>
+      </c>
+      <c r="J220" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="K220" s="2">
+        <v>1</v>
+      </c>
+      <c r="L220" s="2">
+        <v>1</v>
+      </c>
+      <c r="M220" s="2">
+        <v>1</v>
+      </c>
+      <c r="N220" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
         <v>2</v>
       </c>
-      <c r="F220" s="2">
+      <c r="B221" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D221" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F221" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G221" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H221" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="I221" s="2">
+        <v>150000</v>
+      </c>
+      <c r="J221" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="K221" s="2">
         <v>2</v>
       </c>
-      <c r="G220" s="2">
+      <c r="L221" s="2">
         <v>2</v>
       </c>
-      <c r="H220" s="2">
-        <v>150000</v>
-      </c>
-      <c r="I220" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="J220" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A221" s="2">
+      <c r="M221" s="2">
+        <v>2</v>
+      </c>
+      <c r="N221" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
         <v>3</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="D221" s="2"/>
-      <c r="E221" s="2"/>
-      <c r="F221" s="2"/>
-      <c r="G221" s="2"/>
-      <c r="H221" s="2"/>
-      <c r="I221" s="2"/>
-      <c r="J221" s="2"/>
-    </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A222" s="2">
-        <v>4</v>
-      </c>
       <c r="B222" s="2" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
@@ -6259,16 +6305,20 @@
       <c r="H222" s="2"/>
       <c r="I222" s="2"/>
       <c r="J222" s="2"/>
-    </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K222" s="2"/>
+      <c r="L222" s="2"/>
+      <c r="M222" s="2"/>
+      <c r="N222" s="2"/>
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
@@ -6277,616 +6327,630 @@
       <c r="H223" s="2"/>
       <c r="I223" s="2"/>
       <c r="J223" s="2"/>
-    </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A224" s="6"/>
-      <c r="B224" s="6"/>
-      <c r="C224" s="6"/>
-      <c r="D224" s="6"/>
-      <c r="E224" s="6"/>
-      <c r="F224" s="6"/>
-      <c r="G224" s="6"/>
-      <c r="H224" s="6"/>
-      <c r="I224" s="6"/>
-      <c r="J224" s="6"/>
-    </row>
-    <row r="225" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A225" s="9" t="s">
-        <v>612</v>
-      </c>
-      <c r="B225" s="6"/>
-      <c r="C225" s="6"/>
-      <c r="D225" s="6"/>
-      <c r="E225" s="6"/>
-      <c r="F225" s="6"/>
-      <c r="G225" s="6"/>
-      <c r="H225" s="6"/>
-      <c r="I225" s="6"/>
-      <c r="J225" s="6"/>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A226" s="3" t="s">
+      <c r="K223" s="2"/>
+      <c r="L223" s="2"/>
+      <c r="M223" s="2"/>
+      <c r="N223" s="2"/>
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>5</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D224" s="2"/>
+      <c r="E224" s="2"/>
+      <c r="F224" s="2"/>
+      <c r="G224" s="2"/>
+      <c r="H224" s="2"/>
+      <c r="I224" s="2"/>
+      <c r="J224" s="2"/>
+      <c r="K224" s="2"/>
+      <c r="L224" s="2"/>
+      <c r="M224" s="2"/>
+      <c r="N224" s="2"/>
+    </row>
+    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
+        <v>6</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D225" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F225" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="G225" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H225" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="I225" s="2">
+        <v>85000</v>
+      </c>
+      <c r="J225" s="2">
+        <v>45</v>
+      </c>
+      <c r="K225" s="2">
+        <v>11</v>
+      </c>
+      <c r="L225" s="2">
+        <v>25</v>
+      </c>
+      <c r="M225" s="2">
+        <v>8</v>
+      </c>
+      <c r="N225" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A226" s="3"/>
+      <c r="B226" s="3"/>
+      <c r="C226" s="3"/>
+      <c r="D226" s="3"/>
+      <c r="E226" s="3"/>
+      <c r="F226" s="3"/>
+      <c r="G226" s="3"/>
+      <c r="H226" s="3"/>
+      <c r="I226" s="3"/>
+      <c r="J226" s="3"/>
+      <c r="K226" s="3"/>
+      <c r="L226" s="3"/>
+      <c r="M226" s="3"/>
+      <c r="N226" s="3"/>
+    </row>
+    <row r="227" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A227" s="7" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A228" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="B226" s="3" t="s">
+      <c r="B228" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="C226" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="D226" s="3" t="s">
+      <c r="C228" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="D228" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="E226" s="3" t="s">
+      <c r="E228" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="F226" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="G226" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="H226" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="I226" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="J226" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="K226" s="3" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A227" s="2" t="s">
+      <c r="F228" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="G228" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="H228" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="I228" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="J228" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="K228" s="5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="B227" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D227" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E227" s="5">
-        <v>45418</v>
-      </c>
-      <c r="F227" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="G227" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="H227" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="I227" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="J227" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="K227" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A228" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="B228" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E228" s="5">
-        <v>45418</v>
-      </c>
-      <c r="F228" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G228" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="H228" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="I228" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="J228" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="K228" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A229" s="2" t="s">
-        <v>439</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>361</v>
       </c>
       <c r="C229" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D229" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E229" s="6">
+        <v>45418</v>
+      </c>
+      <c r="F229" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="G229" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="D229" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="E229" s="5">
+      <c r="H229" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I229" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="J229" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="K229" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E230" s="6">
         <v>45418</v>
       </c>
-      <c r="F229" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="G229" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="H229" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="I229" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="J229" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="K229" s="2" t="s">
+      <c r="F230" s="2" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A230" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C230" s="2" t="s">
+      <c r="G230" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="D230" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E230" s="5">
-        <v>45418</v>
-      </c>
-      <c r="F230" s="2" t="s">
+      <c r="H230" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="G230" s="2" t="s">
+      <c r="I230" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="H230" s="2" t="s">
+      <c r="J230" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="I230" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J230" s="2" t="s">
+      <c r="K230" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="K230" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>385</v>
+        <v>451</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>361</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E231" s="5">
+        <v>357</v>
+      </c>
+      <c r="E231" s="6">
         <v>45418</v>
       </c>
       <c r="F231" s="2" t="s">
-        <v>434</v>
+        <v>453</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="H231" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I231" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J231" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="K231" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>456</v>
+        <v>382</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>360</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>427</v>
+        <v>457</v>
       </c>
       <c r="D232" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E232" s="6">
+        <v>45418</v>
+      </c>
+      <c r="F232" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="G232" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="H232" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="I232" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="J232" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="K232" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E233" s="6">
+        <v>45418</v>
+      </c>
+      <c r="F233" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="G233" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="H233" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="I233" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="J233" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="K233" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D234" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="E232" s="5">
+      <c r="E234" s="6">
         <v>45462</v>
       </c>
-      <c r="F232" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="G232" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="H232" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="I232" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="J232" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="K232" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A233" s="6"/>
-      <c r="B233" s="6"/>
-      <c r="C233" s="6"/>
-      <c r="D233" s="6"/>
-      <c r="E233" s="7"/>
-      <c r="F233" s="6"/>
-      <c r="G233" s="6"/>
-      <c r="H233" s="6"/>
-      <c r="I233" s="6"/>
-      <c r="J233" s="6"/>
-      <c r="K233" s="6"/>
-    </row>
-    <row r="234" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A234" s="10" t="s">
-        <v>613</v>
-      </c>
-      <c r="B234" s="6"/>
-      <c r="C234" s="6"/>
-      <c r="D234" s="6"/>
-      <c r="E234" s="7"/>
-      <c r="F234" s="6"/>
-      <c r="G234" s="6"/>
-      <c r="H234" s="6"/>
-      <c r="I234" s="6"/>
-      <c r="J234" s="6"/>
-      <c r="K234" s="6"/>
-    </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A235" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="B235" s="3" t="s">
+      <c r="F234" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="G234" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H234" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I234" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="J234" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K234" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A235" s="3"/>
+      <c r="B235" s="3"/>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
+      <c r="E235" s="9"/>
+      <c r="F235" s="3"/>
+      <c r="G235" s="3"/>
+      <c r="H235" s="3"/>
+      <c r="I235" s="3"/>
+      <c r="J235" s="3"/>
+      <c r="K235" s="3"/>
+    </row>
+    <row r="236" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A236" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="B236" s="3"/>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
+      <c r="E236" s="9"/>
+      <c r="F236" s="3"/>
+      <c r="G236" s="3"/>
+      <c r="H236" s="3"/>
+      <c r="I236" s="3"/>
+      <c r="J236" s="3"/>
+      <c r="K236" s="3"/>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A237" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B237" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="C235" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A236" s="2">
+      <c r="C237" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="D237" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
         <v>1</v>
       </c>
-      <c r="B236" s="2">
+      <c r="B238" s="2">
         <v>2</v>
       </c>
-      <c r="C236" s="5">
+      <c r="C238" s="6">
         <v>45419</v>
       </c>
-      <c r="D236" s="2">
+      <c r="D238" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A237" s="6"/>
-      <c r="B237" s="6"/>
-      <c r="C237" s="7"/>
-      <c r="D237" s="6"/>
-    </row>
-    <row r="238" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A238" s="9" t="s">
-        <v>614</v>
-      </c>
-      <c r="B238" s="6"/>
-      <c r="C238" s="7"/>
-      <c r="D238" s="6"/>
-    </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A239" s="3" t="s">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C239" s="1"/>
+    </row>
+    <row r="240" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A240" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="C240" s="1"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B239" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="C239" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="D239" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="E239" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="F239" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="G239" s="3" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A240" s="2">
-        <v>1</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="C240" s="2">
-        <v>4</v>
-      </c>
-      <c r="D240" s="5">
-        <v>45418</v>
-      </c>
-      <c r="E240" s="2">
-        <v>1500</v>
-      </c>
-      <c r="F240" s="2">
-        <v>2024</v>
-      </c>
-      <c r="G240" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A241" s="2">
-        <v>2</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="C241" s="2">
-        <v>14</v>
-      </c>
-      <c r="D241" s="5">
-        <v>45419</v>
-      </c>
-      <c r="E241" s="2">
-        <v>200</v>
-      </c>
-      <c r="F241" s="2">
-        <v>2024</v>
-      </c>
-      <c r="G241" s="2" t="s">
-        <v>469</v>
+      <c r="B241" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C241" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="D241" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="E241" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="F241" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="G241" s="4" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="C242" s="2">
-        <v>1</v>
-      </c>
-      <c r="D242" s="5">
-        <v>45420</v>
+        <v>4</v>
+      </c>
+      <c r="D242" s="6">
+        <v>45418</v>
       </c>
       <c r="E242" s="2">
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="F242" s="2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="G242" s="2" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
-        <v>4</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>472</v>
+        <v>2</v>
+      </c>
+      <c r="B243" s="2">
+        <v>123</v>
       </c>
       <c r="C243" s="2">
-        <v>5</v>
-      </c>
-      <c r="D243" s="5">
-        <v>45421</v>
+        <v>14</v>
+      </c>
+      <c r="D243" s="6">
+        <v>45419</v>
       </c>
       <c r="E243" s="2">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="F243" s="2">
         <v>2024</v>
       </c>
       <c r="G243" s="2" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="C244" s="2">
-        <v>12</v>
-      </c>
-      <c r="D244" s="5">
-        <v>45422</v>
+        <v>1</v>
+      </c>
+      <c r="D244" s="6">
+        <v>45420</v>
       </c>
       <c r="E244" s="2">
-        <v>100</v>
+        <v>1250</v>
       </c>
       <c r="F244" s="2">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="G244" s="2" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>471</v>
+        <v>482</v>
       </c>
       <c r="C245" s="2">
-        <v>2</v>
-      </c>
-      <c r="D245" s="5">
-        <v>45419</v>
+        <v>5</v>
+      </c>
+      <c r="D245" s="6">
+        <v>45421</v>
       </c>
       <c r="E245" s="2">
-        <v>850</v>
+        <v>700</v>
       </c>
       <c r="F245" s="2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="G245" s="2" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="C246" s="2">
-        <v>15</v>
-      </c>
-      <c r="D246" s="5">
-        <v>45420</v>
+        <v>12</v>
+      </c>
+      <c r="D246" s="6">
+        <v>45422</v>
       </c>
       <c r="E246" s="2">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="F246" s="2">
         <v>2024</v>
       </c>
       <c r="G246" s="2" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="C247" s="2">
-        <v>3</v>
-      </c>
-      <c r="D247" s="5">
-        <v>45418</v>
+        <v>2</v>
+      </c>
+      <c r="D247" s="6">
+        <v>45419</v>
       </c>
       <c r="E247" s="2">
-        <v>1500</v>
+        <v>850</v>
       </c>
       <c r="F247" s="2">
         <v>2023</v>
       </c>
       <c r="G247" s="2" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="C248" s="2">
-        <v>10</v>
-      </c>
-      <c r="D248" s="5">
-        <v>45419</v>
+        <v>15</v>
+      </c>
+      <c r="D248" s="6">
+        <v>45420</v>
       </c>
       <c r="E248" s="2">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="F248" s="2">
         <v>2024</v>
       </c>
-      <c r="G248" s="2">
-        <v>2</v>
+      <c r="G248" s="2" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C249" s="2">
-        <v>11</v>
-      </c>
-      <c r="D249" s="5">
+        <v>3</v>
+      </c>
+      <c r="D249" s="6">
         <v>45418</v>
       </c>
       <c r="E249" s="2">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F249" s="2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G249" s="2" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="C250" s="2">
-        <v>9</v>
-      </c>
-      <c r="D250" s="5">
-        <v>45414</v>
+        <v>10</v>
+      </c>
+      <c r="D250" s="6">
+        <v>45419</v>
       </c>
       <c r="E250" s="2">
-        <v>70</v>
+        <v>450</v>
       </c>
       <c r="F250" s="2">
         <v>2024</v>
@@ -6897,292 +6961,303 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
+        <v>10</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C251" s="2">
+        <v>11</v>
+      </c>
+      <c r="D251" s="6">
+        <v>45418</v>
+      </c>
+      <c r="E251" s="2">
+        <v>300</v>
+      </c>
+      <c r="F251" s="2">
+        <v>2022</v>
+      </c>
+      <c r="G251" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>12</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C252" s="2">
+        <v>9</v>
+      </c>
+      <c r="D252" s="6">
+        <v>45414</v>
+      </c>
+      <c r="E252" s="2">
+        <v>70</v>
+      </c>
+      <c r="F252" s="2">
+        <v>2024</v>
+      </c>
+      <c r="G252" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
         <v>13</v>
       </c>
-      <c r="B251" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="C251" s="2">
-        <v>5</v>
-      </c>
-      <c r="D251" s="5">
+      <c r="B253" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C253" s="2">
+        <v>6</v>
+      </c>
+      <c r="D253" s="6">
         <v>45420</v>
       </c>
-      <c r="E251" s="2">
+      <c r="E253" s="2">
         <v>900</v>
       </c>
-      <c r="F251" s="2">
+      <c r="F253" s="2">
         <v>2023</v>
       </c>
-      <c r="G251" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A252" s="6"/>
-      <c r="B252" s="6"/>
-      <c r="C252" s="6"/>
-      <c r="D252" s="7"/>
-      <c r="E252" s="6"/>
-      <c r="F252" s="6"/>
-      <c r="G252" s="6"/>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="8" t="s">
-        <v>615</v>
-      </c>
-      <c r="B253" s="6"/>
-      <c r="C253" s="6"/>
-      <c r="D253" s="7"/>
-      <c r="E253" s="6"/>
-      <c r="F253" s="6"/>
-      <c r="G253" s="6"/>
+      <c r="G253" s="2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="C254" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="D254" s="3" t="s">
-        <v>479</v>
+      <c r="A254" s="2">
+        <v>14</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C254" s="2">
+        <v>37</v>
+      </c>
+      <c r="D254" s="6">
+        <v>45450</v>
+      </c>
+      <c r="E254" s="2">
+        <v>300</v>
+      </c>
+      <c r="F254" s="2">
+        <v>2023</v>
+      </c>
+      <c r="G254" s="2" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A255" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="B255" s="5">
-        <v>45292</v>
-      </c>
-      <c r="C255" s="5">
-        <v>45382</v>
-      </c>
-      <c r="D255" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A256" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="B256" s="5">
-        <v>45306</v>
-      </c>
-      <c r="C256" s="5">
-        <v>45352</v>
-      </c>
-      <c r="D256" s="2">
-        <v>0.05</v>
-      </c>
+      <c r="D255" s="1"/>
+    </row>
+    <row r="256" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A256" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="D256" s="1"/>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A257" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="B257" s="5">
-        <v>45292</v>
-      </c>
-      <c r="C257" s="5">
-        <v>45382</v>
-      </c>
-      <c r="D257" s="2">
-        <v>0.05</v>
+      <c r="A257" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="D257" s="4" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="B258" s="5">
+        <v>490</v>
+      </c>
+      <c r="B258" s="6">
         <v>45292</v>
       </c>
-      <c r="C258" s="5">
-        <v>45322</v>
+      <c r="C258" s="6">
+        <v>45382</v>
       </c>
       <c r="D258" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="B259" s="5">
+        <v>491</v>
+      </c>
+      <c r="B259" s="6">
+        <v>45306</v>
+      </c>
+      <c r="C259" s="6">
+        <v>45352</v>
+      </c>
+      <c r="D259" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B260" s="6">
         <v>45292</v>
       </c>
-      <c r="C259" s="5">
+      <c r="C260" s="6">
+        <v>45382</v>
+      </c>
+      <c r="D260" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B261" s="6">
+        <v>45292</v>
+      </c>
+      <c r="C261" s="6">
         <v>45322</v>
       </c>
-      <c r="D259" s="2">
+      <c r="D261" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B262" s="6">
+        <v>45292</v>
+      </c>
+      <c r="C262" s="6">
+        <v>45322</v>
+      </c>
+      <c r="D262" s="2">
         <v>0.08</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A260" s="6"/>
-      <c r="B260" s="7"/>
-      <c r="C260" s="7"/>
-      <c r="D260" s="6"/>
-    </row>
-    <row r="261" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A261" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="B261" s="7"/>
-      <c r="C261" s="7"/>
-      <c r="D261" s="6"/>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A262" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A263" s="2">
-        <v>1</v>
-      </c>
-      <c r="B263" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A264" s="2">
-        <v>2</v>
-      </c>
-      <c r="B264" s="2" t="s">
-        <v>440</v>
-      </c>
+      <c r="A263" s="3"/>
+      <c r="B263" s="9"/>
+      <c r="C263" s="9"/>
+      <c r="D263" s="3"/>
+    </row>
+    <row r="264" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A264" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="B264" s="9"/>
+      <c r="C264" s="9"/>
+      <c r="D264" s="3"/>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A265" s="2">
-        <v>3</v>
-      </c>
-      <c r="B265" s="2" t="s">
-        <v>486</v>
+      <c r="A265" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>487</v>
+        <v>452</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>446</v>
+        <v>462</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
+        <v>5</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="2">
+        <v>6</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>7</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="2">
         <v>8</v>
       </c>
-      <c r="B270" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="6"/>
-      <c r="B271" s="6"/>
-    </row>
-    <row r="272" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A272" s="9" t="s">
-        <v>617</v>
-      </c>
-      <c r="B272" s="6"/>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A273" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="B273" s="3" t="s">
+      <c r="B273" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A275" s="10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B276" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="C273" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="D273" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A274" s="2">
-        <v>1</v>
-      </c>
-      <c r="B274" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="C274" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="D274" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A275" s="2">
-        <v>2</v>
-      </c>
-      <c r="B275" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C275" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="D275" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A276" s="2">
-        <v>3</v>
-      </c>
-      <c r="B276" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C276" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="D276" s="2" t="s">
-        <v>395</v>
+      <c r="C276" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="D276" s="4" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>494</v>
+        <v>414</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>396</v>
@@ -7190,820 +7265,984 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>418</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>493</v>
+        <v>414</v>
       </c>
       <c r="D278" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="2">
+        <v>3</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D279" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="2">
+        <v>4</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="D280" s="2" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="6"/>
-      <c r="B279" s="6"/>
-      <c r="C279" s="6"/>
-      <c r="D279" s="6"/>
-    </row>
-    <row r="280" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A280" s="9" t="s">
-        <v>619</v>
-      </c>
-      <c r="B280" s="6"/>
-      <c r="C280" s="6"/>
-      <c r="D280" s="6"/>
-    </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="B281" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="C281" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="D281" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" s="2">
-        <v>1</v>
-      </c>
-      <c r="B282" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C282" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="D282" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="2">
-        <v>2</v>
-      </c>
-      <c r="B283" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C283" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="D283" s="2">
-        <v>2</v>
+      <c r="A281" s="2">
+        <v>5</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D281" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A283" s="10" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A284" s="2">
-        <v>3</v>
-      </c>
-      <c r="B284" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C284" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="D284" s="2">
-        <v>3</v>
+      <c r="A284" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B284" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C284" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="D284" s="4" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="D285" s="2">
-        <v>4</v>
+        <v>490</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="D286" s="2">
-        <v>5</v>
+        <v>490</v>
+      </c>
+      <c r="D286" s="2" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="D287" s="2">
-        <v>1</v>
+        <v>490</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="2">
+        <v>4</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D288" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="2">
+        <v>5</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D289" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="2">
+        <v>6</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="2">
         <v>7</v>
       </c>
-      <c r="B288" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="D288" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A289" s="2">
+      <c r="B291" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D291" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="2">
         <v>8</v>
       </c>
-      <c r="B289" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C289" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="D289" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A290" s="2">
+      <c r="B292" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D292" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="2">
         <v>9</v>
       </c>
-      <c r="B290" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C290" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="D290" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A291" s="2">
+      <c r="B293" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D293" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="2">
         <v>10</v>
       </c>
-      <c r="B291" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="C291" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="D291" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A292" s="2">
+      <c r="B294" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="2">
         <v>11</v>
       </c>
-      <c r="B292" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="D292" s="2" t="s">
+      <c r="B295" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D295" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A293" s="2">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="2">
         <v>12</v>
       </c>
-      <c r="B293" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="D293" s="2" t="s">
+      <c r="B296" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D296" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A294" s="2">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="2">
         <v>13</v>
       </c>
-      <c r="B294" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="C294" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="D294" s="2">
+      <c r="B297" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D297" s="2">
         <v>9874</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A295" s="2">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="2">
         <v>14</v>
       </c>
-      <c r="B295" s="2">
+      <c r="B298" s="2">
         <v>123</v>
       </c>
-      <c r="C295" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="D295" s="2">
+      <c r="C298" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D298" s="2">
         <v>1152</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A296" s="2">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="2">
         <v>15</v>
       </c>
-      <c r="B296" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="C296" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="D296" s="2" t="s">
+      <c r="B299" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D299" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A297" s="2">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="2">
         <v>16</v>
       </c>
-      <c r="B297" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="D297" s="2">
+      <c r="B300" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D300" s="2">
         <v>9156</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A298" s="2">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="2">
         <v>19</v>
       </c>
-      <c r="B298" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="C298" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="D298" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A299" s="6"/>
-      <c r="B299" s="6"/>
-      <c r="C299" s="6"/>
-      <c r="D299" s="6"/>
-    </row>
-    <row r="300" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A300" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="B300" s="6"/>
-      <c r="C300" s="6"/>
-      <c r="D300" s="6"/>
-    </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A301" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="B301" s="3" t="s">
+      <c r="B301" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C301" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="C301" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="D301" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="E301" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="F301" s="3" t="s">
+      <c r="D301" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="2">
+        <v>22</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D302" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="2">
+        <v>23</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C303" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D303" s="2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="2">
+        <v>24</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D304" s="2" t="s">
         <v>509</v>
-      </c>
-      <c r="G301" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="H301" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="I301" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="J301" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="K301" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="L301" s="3" t="s">
-        <v>515</v>
-      </c>
-      <c r="M301" s="3" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A302" s="2">
-        <v>23</v>
-      </c>
-      <c r="B302" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="C302" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="D302" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E302" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="F302" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="G302" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="H302" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="I302" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="J302" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="K302" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="L302" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="M302" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A303" s="2">
-        <v>2</v>
-      </c>
-      <c r="B303" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="C303" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="D303" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="E303" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="F303" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="G303" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="H303" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="I303" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="J303" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="K303" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="L303" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M303" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A304" s="2">
-        <v>4</v>
-      </c>
-      <c r="B304" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="C304" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="D304" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="E304" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="F304" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="G304" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="H304" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="I304" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="J304" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="K304" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="L304" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M304" s="2" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="305" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A305" s="2">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>545</v>
+        <v>484</v>
       </c>
       <c r="C305" s="2" t="s">
-        <v>546</v>
+        <v>490</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="E305" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="F305" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="G305" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="H305" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="I305" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="J305" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="K305" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="L305" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="M305" s="2" t="s">
-        <v>355</v>
+        <v>427</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A306" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>554</v>
+        <v>485</v>
       </c>
       <c r="C306" s="2" t="s">
-        <v>555</v>
+        <v>403</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E306" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="F306" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="G306" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="H306" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="I306" s="2"/>
-      <c r="J306" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="K306" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="L306" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M306" s="2" t="s">
-        <v>355</v>
+        <v>427</v>
       </c>
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A307" s="2">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>560</v>
+        <v>484</v>
       </c>
       <c r="C307" s="2" t="s">
-        <v>561</v>
+        <v>403</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="E307" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="F307" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="G307" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="H307" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="I307" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="J307" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="K307" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="L307" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M307" s="2"/>
+        <v>427</v>
+      </c>
     </row>
     <row r="308" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A308" s="2">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>569</v>
+        <v>485</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>570</v>
+        <v>490</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E308" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="F308" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="G308" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="H308" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="I308" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="J308" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="K308" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="L308" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M308" s="2" t="s">
-        <v>355</v>
+        <v>427</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A309" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>577</v>
+        <v>485</v>
       </c>
       <c r="C309" s="2" t="s">
-        <v>578</v>
+        <v>506</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="E309" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="F309" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="G309" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="H309" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="I309" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="J309" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="K309" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="L309" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M309" s="2" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A310" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>582</v>
+        <v>482</v>
       </c>
       <c r="C310" s="2" t="s">
-        <v>583</v>
+        <v>490</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E310" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="F310" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="G310" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="H310" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="I310" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="J310" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="K310" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="L310" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="M310" s="2" t="s">
-        <v>355</v>
+        <v>427</v>
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A311" s="2">
+        <v>36</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C311" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D311" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A313" s="7" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A314" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="B314" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C314" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D314" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="E314" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="F314" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="G314" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="H314" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="I314" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="J314" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="K314" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="L314" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="M314" s="4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A315" s="2">
+        <v>23</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C315" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D315" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E315" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="F315" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="G315" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="H315" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="I315" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="J315" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="K315" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="L315" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="M315" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A316" s="2">
+        <v>2</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D316" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E316" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="F316" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="G316" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="H316" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="I316" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="J316" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="K316" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="L316" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M316" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A317" s="2">
+        <v>4</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C317" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="D317" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="E317" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F317" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="G317" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="H317" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="I317" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="J317" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="K317" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="L317" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M317" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A318" s="2">
+        <v>3</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C318" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D318" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E318" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F318" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="G318" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H318" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="I318" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="J318" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="K318" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="L318" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="M318" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A319" s="2">
+        <v>24</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="D319" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E319" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="F319" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="G319" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="H319" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="I319" s="2"/>
+      <c r="J319" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="K319" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="L319" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M319" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A320" s="2">
+        <v>1</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D320" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="E320" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F320" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="G320" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="H320" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="I320" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="J320" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="K320" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="L320" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M320" s="2"/>
+    </row>
+    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A321" s="2">
+        <v>19</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="D321" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E321" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="F321" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="G321" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="H321" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="I321" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J321" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="K321" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="L321" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M321" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A322" s="2">
+        <v>31</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="D322" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="E322" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="F322" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="G322" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="H322" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="I322" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="J322" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="K322" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="L322" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M322" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A323" s="2">
+        <v>34</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D323" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E323" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="F323" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G323" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="H323" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I323" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="J323" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="K323" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="L323" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="M323" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A324" s="2">
         <v>37</v>
       </c>
-      <c r="B311" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="C311" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="D311" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E311" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="F311" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="G311" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="H311" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="I311" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="J311" s="2" t="s">
+      <c r="B324" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="K311" s="2" t="s">
+      <c r="C324" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="L311" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M311" s="2" t="s">
+      <c r="D324" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E324" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="F324" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="G324" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="H324" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="I324" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="J324" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="K324" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="L324" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M324" s="2" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A312" s="2">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A325" s="2">
         <v>40</v>
       </c>
-      <c r="B312" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="C312" s="2" t="s">
+      <c r="B325" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D325" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E325" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="F325" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="G325" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="H325" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="D312" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E312" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="F312" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="G312" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="H312" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="I312" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="J312" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="K312" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="L312" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="M312" s="2" t="s">
+      <c r="I325" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="J325" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="K325" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="L325" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="M325" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A313" s="2">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A326" s="2">
         <v>41</v>
       </c>
-      <c r="B313" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="C313" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="D313" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="E313" s="2">
+      <c r="B326" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="D326" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E326" s="2">
         <v>123</v>
       </c>
-      <c r="F313" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="G313" s="2"/>
-      <c r="H313" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="I313" s="2"/>
-      <c r="J313" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="K313" s="2">
+      <c r="F326" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="G326" s="2"/>
+      <c r="H326" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="I326" s="2"/>
+      <c r="J326" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="K326" s="2">
         <v>123123123</v>
       </c>
-      <c r="L313" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="M313" s="2" t="s">
+      <c r="L326" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="M326" s="2" t="s">
         <v>355</v>
       </c>
     </row>

</xml_diff>